<commit_message>
Made some updates to bump chart
</commit_message>
<xml_diff>
--- a/subscriber_counts.xlsx
+++ b/subscriber_counts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e4c8cbec7ccee8f/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moon1\Desktop\D-D-D-Data-Dazzlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50941436-5C5E-4812-9FB0-8F763C26CE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC30BA6-2276-46E4-BC9A-4E7C8268F3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B775F0B6-5D69-4CC7-8348-DB87AF3AFD52}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="10008" xr2:uid="{B775F0B6-5D69-4CC7-8348-DB87AF3AFD52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Subscrition Service</t>
-  </si>
-  <si>
     <t>Revenue ($bn)</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Tubi</t>
+  </si>
+  <si>
+    <t>Streaming Service</t>
   </si>
 </sst>
 </file>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180C4FE8-137D-48F9-B821-14C09335DA16}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,13 +455,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
         <v>2011</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>3.1</v>
@@ -483,7 +483,7 @@
         <v>2012</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>3.5</v>
@@ -497,7 +497,7 @@
         <v>2013</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>4.5</v>
@@ -511,7 +511,7 @@
         <v>2014</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>5.4</v>
@@ -525,7 +525,7 @@
         <v>2015</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>6.7</v>
@@ -539,7 +539,7 @@
         <v>2016</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>8.8000000000000007</v>
@@ -553,7 +553,7 @@
         <v>2017</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>11.6</v>
@@ -567,7 +567,7 @@
         <v>2018</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>15.7</v>
@@ -581,7 +581,7 @@
         <v>2019</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>20.100000000000001</v>
@@ -595,7 +595,7 @@
         <v>2020</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>24.9</v>
@@ -609,7 +609,7 @@
         <v>2021</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>29.6</v>
@@ -623,7 +623,7 @@
         <v>2022</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>31.6</v>
@@ -637,7 +637,7 @@
         <v>2023</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>33.700000000000003</v>
@@ -651,7 +651,7 @@
         <v>2024</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>39</v>
@@ -665,7 +665,7 @@
         <v>2011</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>0.4</v>
@@ -679,7 +679,7 @@
         <v>2012</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0.6</v>
@@ -693,7 +693,7 @@
         <v>2013</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>1.1000000000000001</v>
@@ -707,7 +707,7 @@
         <v>2014</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>1.6</v>
@@ -721,7 +721,7 @@
         <v>2015</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -735,7 +735,7 @@
         <v>2016</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>2.4</v>
@@ -749,7 +749,7 @@
         <v>2017</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>3.1</v>
@@ -763,7 +763,7 @@
         <v>2018</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>3.5</v>
@@ -777,7 +777,7 @@
         <v>2019</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>4.5</v>
@@ -791,7 +791,7 @@
         <v>2020</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>7.2</v>
@@ -805,7 +805,7 @@
         <v>2021</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>9.6</v>
@@ -819,7 +819,7 @@
         <v>2022</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>10.7</v>
@@ -833,7 +833,7 @@
         <v>2023</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>11.2</v>
@@ -847,7 +847,7 @@
         <v>2024</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -861,7 +861,7 @@
         <v>2020</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <v>0.11990000000000001</v>
@@ -875,7 +875,7 @@
         <v>2021</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>0.52649999999999997</v>
@@ -889,7 +889,7 @@
         <v>2022</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>0.53449999999999998</v>
@@ -903,7 +903,7 @@
         <v>2023</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <v>0.499</v>
@@ -917,7 +917,7 @@
         <v>2020</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <v>2.8</v>
@@ -931,7 +931,7 @@
         <v>2021</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35">
         <v>5.2</v>
@@ -945,7 +945,7 @@
         <v>2022</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36">
         <v>7.4</v>
@@ -959,7 +959,7 @@
         <v>2023</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37">
         <v>8.4</v>
@@ -973,7 +973,7 @@
         <v>2024</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C38">
         <v>10.4</v>
@@ -987,7 +987,7 @@
         <v>2019</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39">
         <v>5.4</v>
@@ -1001,7 +1001,7 @@
         <v>2020</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40">
         <v>7.8</v>
@@ -1015,7 +1015,7 @@
         <v>2021</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41">
         <v>11.3</v>
@@ -1029,7 +1029,7 @@
         <v>2022</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42">
         <v>12.5</v>
@@ -1043,7 +1043,7 @@
         <v>2023</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>14</v>
@@ -1057,7 +1057,7 @@
         <v>2024</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D44">
         <v>290</v>
@@ -1068,7 +1068,7 @@
         <v>2019</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <v>0.15</v>
@@ -1082,7 +1082,7 @@
         <v>2020</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46">
         <v>0.25</v>
@@ -1096,7 +1096,7 @@
         <v>2021</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C47">
         <v>0.38</v>
@@ -1110,7 +1110,7 @@
         <v>2022</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48">
         <v>0.77500000000000002</v>
@@ -1124,7 +1124,7 @@
         <v>2023</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49">
         <v>0.9</v>
@@ -1138,7 +1138,7 @@
         <v>2024</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50">
         <v>78</v>

</xml_diff>